<commit_message>
Premiers prix pour CNC mill
</commit_message>
<xml_diff>
--- a/CR - Cost Report/CBOM/Cost.xlsx
+++ b/CR - Cost Report/CBOM/Cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\OneDrive\Documents\EPSA\Optipute\CR - Cost Report\CBOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3308F9AE-B14A-4CDA-9429-7A2F57E33A6B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886D43F4-2627-488D-9C90-9837A1E61B47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE75819C-F2BF-48A4-A25A-3F0C921A5E1F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="358">
   <si>
     <t>Alu 7075 T6</t>
   </si>
@@ -882,9 +882,6 @@
     <t>Volume/time</t>
   </si>
   <si>
-    <t xml:space="preserve">Tool sample and ponderate mean /time </t>
-  </si>
-  <si>
     <t>5 % of initial cost /year</t>
   </si>
   <si>
@@ -1084,6 +1081,39 @@
   </si>
   <si>
     <t>Electricity consumption for office and small components (avg 16kW)</t>
+  </si>
+  <si>
+    <t>https://www.fournisseurs-electricite.com/edf/pro/tarifs-reglementes/jaune#decomposition-facture</t>
+  </si>
+  <si>
+    <t>https://www.fournisseurs-electricite.com/guides/compteur/puissance/estimation?fbclid=IwAR0M9rlabDNFJxLa_aehdEGtK33qlQUwFO2xf_a1OlrFo_cEoo8_Df1M5hg</t>
+  </si>
+  <si>
+    <t>€/hour</t>
+  </si>
+  <si>
+    <t>Cost/hour running</t>
+  </si>
+  <si>
+    <t>Cost of machining part (€/mm^3)</t>
+  </si>
+  <si>
+    <t>Cost of Setup</t>
+  </si>
+  <si>
+    <t>Cost of programing part Technician(€/mm^3)</t>
+  </si>
+  <si>
+    <t>Cost of programing part Engineer (€/mm^3)</t>
+  </si>
+  <si>
+    <t>Cost of programing part Operator (€/mm^3)</t>
+  </si>
+  <si>
+    <t>Fixed cost</t>
+  </si>
+  <si>
+    <t>Fixed cost/hour to charge on operation (machine/station/programing/metrology)</t>
   </si>
 </sst>
 </file>
@@ -1268,7 +1298,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1357,6 +1387,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="12" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1375,16 +1420,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="12" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1704,10 +1740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371D2E59-26F6-41B6-8D22-66B526DB6BB8}">
-  <dimension ref="A1:V57"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,33 +1766,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
       <c r="M1" s="34"/>
       <c r="N1" s="34"/>
-      <c r="P1" s="45" t="s">
+      <c r="P1" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="T1" s="47" t="s">
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="T1" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
     </row>
     <row r="2" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1833,10 +1869,10 @@
         <f>C3/D3</f>
         <v>232</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="49"/>
+      <c r="H3" s="54"/>
       <c r="I3" t="s">
         <v>266</v>
       </c>
@@ -1881,7 +1917,7 @@
         <v>183.84</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H4" s="9">
         <v>22.4</v>
@@ -1928,7 +1964,7 @@
         <v>127.2</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H5" s="40">
         <f>C49</f>
@@ -1975,7 +2011,7 @@
         <v>4833.4809999999998</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H6" s="9">
         <v>15</v>
@@ -1987,7 +2023,7 @@
         <v>271</v>
       </c>
       <c r="K6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L6" s="24">
         <f>0.05*L3</f>
@@ -2022,9 +2058,9 @@
         <v>320.96000000000004</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="H7" s="50">
+        <v>313</v>
+      </c>
+      <c r="H7" s="45">
         <f>1/10000</f>
         <v>1E-4</v>
       </c>
@@ -2035,7 +2071,7 @@
         <v>272</v>
       </c>
       <c r="K7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L7" s="33">
         <f>H4*0.8*C53</f>
@@ -2060,9 +2096,9 @@
         <v>49.290039304557205</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="H8" s="50">
+        <v>314</v>
+      </c>
+      <c r="H8" s="45">
         <f>H7*0.4</f>
         <v>4.0000000000000003E-5</v>
       </c>
@@ -2080,7 +2116,7 @@
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C9" s="24">
         <f>Metrology!E25</f>
@@ -2094,10 +2130,22 @@
         <v>539</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H9" s="9">
         <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>275</v>
+      </c>
+      <c r="J9" t="s">
+        <v>272</v>
+      </c>
+      <c r="K9" t="s">
+        <v>349</v>
+      </c>
+      <c r="L9" s="2">
+        <v>20</v>
       </c>
       <c r="P9" s="14"/>
     </row>
@@ -2110,9 +2158,9 @@
       </c>
       <c r="E10" s="25"/>
       <c r="G10" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="H10" s="53">
+        <v>316</v>
+      </c>
+      <c r="H10" s="48">
         <f>SUM(N3:N6)</f>
         <v>16773</v>
       </c>
@@ -2133,10 +2181,10 @@
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="43" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C11" s="24">
-        <f>Energies!B5</f>
+        <f>Energies!B6</f>
         <v>2843.9040000000005</v>
       </c>
       <c r="D11">
@@ -2147,11 +2195,11 @@
         <v>2843.9040000000005</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="H11" s="53">
-        <f>H10/(H5*C47*C48)</f>
-        <v>14.012531328320803</v>
+        <v>317</v>
+      </c>
+      <c r="H11" s="48">
+        <f>H10/(H5*C47*C48)+C59</f>
+        <v>26.510226878703875</v>
       </c>
       <c r="P11" s="15" t="s">
         <v>69</v>
@@ -2163,7 +2211,7 @@
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="43" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C12" s="2">
         <f>16*C47*C48*C53</f>
@@ -2176,16 +2224,12 @@
         <f t="shared" si="0"/>
         <v>1999.4687999999999</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" t="s">
-        <v>275</v>
-      </c>
-      <c r="J12" t="s">
-        <v>272</v>
-      </c>
-      <c r="K12" t="s">
-        <v>280</v>
+      <c r="G12" s="44" t="s">
+        <v>350</v>
+      </c>
+      <c r="H12" s="48">
+        <f>H11+L10+L9+L7</f>
+        <v>47.913362878703872</v>
       </c>
       <c r="P12" s="18"/>
       <c r="Q12" t="s">
@@ -2202,19 +2246,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" t="s">
-        <v>271</v>
-      </c>
-      <c r="M13">
-        <v>10</v>
-      </c>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
@@ -2228,11 +2261,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" t="s">
-        <v>22</v>
-      </c>
+      <c r="G14" s="44" t="s">
+        <v>351</v>
+      </c>
+      <c r="H14" s="45">
+        <f>(Manpower!H5+H12)*H7/60</f>
+        <v>1.0217807764662842E-4</v>
+      </c>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
@@ -2246,10 +2282,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="51"/>
-      <c r="I15" t="s">
-        <v>19</v>
+      <c r="G15" s="44" t="s">
+        <v>355</v>
+      </c>
+      <c r="H15" s="55">
+        <f>(Manpower!H5)*H8/60</f>
+        <v>8.9289891395154577E-6</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -2258,10 +2296,12 @@
         <v>48</v>
       </c>
       <c r="E16" s="25"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" t="s">
-        <v>23</v>
+      <c r="G16" s="44" t="s">
+        <v>353</v>
+      </c>
+      <c r="H16" s="55">
+        <f>(Manpower!H6)*H8/60</f>
+        <v>1.6628654970760235E-5</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -2276,10 +2316,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="52"/>
-      <c r="I17" t="s">
-        <v>24</v>
+      <c r="G17" s="44" t="s">
+        <v>354</v>
+      </c>
+      <c r="H17" s="55">
+        <f>(Manpower!H7)*H8/60</f>
+        <v>2.9174185463659156E-5</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -2294,15 +2336,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="52"/>
-      <c r="I18" t="s">
-        <v>27</v>
+      <c r="G18" s="44" t="s">
+        <v>352</v>
+      </c>
+      <c r="H18" s="48">
+        <f>(Manpower!H5+H11)*H9/60</f>
+        <v>9.9759276469942666</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B19" t="s">
         <v>189</v>
@@ -2318,16 +2362,24 @@
         <f t="shared" si="0"/>
         <v>39809</v>
       </c>
-      <c r="G19" s="10"/>
+      <c r="G19" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H19" s="10"/>
       <c r="I19" t="s">
-        <v>61</v>
+        <v>21</v>
+      </c>
+      <c r="J19" t="s">
+        <v>271</v>
+      </c>
+      <c r="M19">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C20" s="24">
         <f>C45*0.4</f>
@@ -2340,18 +2392,16 @@
         <f t="shared" si="0"/>
         <v>27937.200000000001</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="11"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
       <c r="I20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C21" s="24">
         <f>Manpower!G8</f>
@@ -2364,16 +2414,16 @@
         <f t="shared" si="0"/>
         <v>24683.68</v>
       </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="46"/>
       <c r="I21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C22" s="24">
         <f>Manpower!B30</f>
@@ -2386,10 +2436,10 @@
         <f t="shared" si="0"/>
         <v>13716.36</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
       <c r="I22" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -2410,10 +2460,10 @@
         <f t="shared" si="0"/>
         <v>959.37599999999998</v>
       </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="47"/>
       <c r="I23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -2432,10 +2482,10 @@
         <f t="shared" si="0"/>
         <v>38.591999999999999</v>
       </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="47"/>
       <c r="I24" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -2454,26 +2504,10 @@
         <f t="shared" si="0"/>
         <v>277.54199999999997</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25" s="9"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
       <c r="I25" t="s">
-        <v>304</v>
-      </c>
-      <c r="J25" t="s">
-        <v>271</v>
-      </c>
-      <c r="L25" s="24">
-        <f>'TIG Welder'!F2+'TIG Welder'!F3</f>
-        <v>5308.6</v>
-      </c>
-      <c r="M25">
-        <v>10</v>
-      </c>
-      <c r="N25" s="24">
-        <f>L25/M25</f>
-        <v>530.86</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -2492,24 +2526,12 @@
         <f t="shared" si="0"/>
         <v>316.8</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="G26" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="11"/>
       <c r="I26" t="s">
-        <v>57</v>
-      </c>
-      <c r="J26" t="s">
-        <v>271</v>
-      </c>
-      <c r="L26" s="24">
-        <f>'TIG Welder'!F4</f>
-        <v>3859.6</v>
-      </c>
-      <c r="M26">
-        <v>10</v>
-      </c>
-      <c r="N26" s="24">
-        <f t="shared" ref="N26:N30" si="2">L26/M26</f>
-        <v>385.96</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -2528,24 +2550,10 @@
         <f t="shared" si="0"/>
         <v>796.80000000000007</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
       <c r="I27" t="s">
-        <v>309</v>
-      </c>
-      <c r="J27" t="s">
-        <v>271</v>
-      </c>
-      <c r="L27" s="24">
-        <f>'TIG Welder'!F6</f>
-        <v>146</v>
-      </c>
-      <c r="M27">
-        <v>5</v>
-      </c>
-      <c r="N27" s="24">
-        <f t="shared" si="2"/>
-        <v>29.2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -2564,24 +2572,10 @@
         <f t="shared" si="0"/>
         <v>1224</v>
       </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
       <c r="I28" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" t="s">
-        <v>271</v>
-      </c>
-      <c r="L28" s="24">
-        <f>'TIG Welder'!F6+'TIG Welder'!F7</f>
-        <v>196</v>
-      </c>
-      <c r="M28">
-        <v>2</v>
-      </c>
-      <c r="N28" s="24">
-        <f t="shared" si="2"/>
-        <v>98</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2596,24 +2590,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
       <c r="I29" t="s">
-        <v>294</v>
-      </c>
-      <c r="J29" t="s">
-        <v>271</v>
-      </c>
-      <c r="L29" s="24">
-        <f>'TIG Welder'!F5</f>
-        <v>8579</v>
-      </c>
-      <c r="M29">
-        <v>10</v>
-      </c>
-      <c r="N29" s="24">
-        <f t="shared" si="2"/>
-        <v>857.9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -2630,27 +2610,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
       <c r="I30" t="s">
-        <v>27</v>
-      </c>
-      <c r="J30" t="s">
-        <v>271</v>
-      </c>
-      <c r="K30" t="s">
-        <v>308</v>
-      </c>
-      <c r="L30" s="24">
-        <f>0.03*(L25+L26)</f>
-        <v>275.04599999999999</v>
-      </c>
-      <c r="M30">
-        <v>1</v>
-      </c>
-      <c r="N30" s="24">
-        <f t="shared" si="2"/>
-        <v>275.04599999999999</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -2665,16 +2628,26 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G31" s="9"/>
+      <c r="G31" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="H31" s="9"/>
       <c r="I31" t="s">
-        <v>24</v>
+        <v>303</v>
       </c>
       <c r="J31" t="s">
-        <v>272</v>
-      </c>
-      <c r="K31" t="s">
-        <v>277</v>
+        <v>271</v>
+      </c>
+      <c r="L31" s="24">
+        <f>'TIG Welder'!F2+'TIG Welder'!F3</f>
+        <v>5308.6</v>
+      </c>
+      <c r="M31">
+        <v>10</v>
+      </c>
+      <c r="N31" s="24">
+        <f>L31/M31</f>
+        <v>530.86</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2686,19 +2659,27 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
       <c r="I32" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="J32" t="s">
-        <v>272</v>
-      </c>
-      <c r="K32" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+      <c r="L32" s="24">
+        <f>'TIG Welder'!F4</f>
+        <v>3859.6</v>
+      </c>
+      <c r="M32">
+        <v>10</v>
+      </c>
+      <c r="N32" s="24">
+        <f t="shared" ref="N32:N36" si="2">L32/M32</f>
+        <v>385.96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" t="s">
         <v>56</v>
@@ -2710,19 +2691,27 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
       <c r="I33" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="J33" t="s">
-        <v>272</v>
-      </c>
-      <c r="K33" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+      <c r="L33" s="24">
+        <f>'TIG Welder'!F6</f>
+        <v>146</v>
+      </c>
+      <c r="M33">
+        <v>5</v>
+      </c>
+      <c r="N33" s="24">
+        <f t="shared" si="2"/>
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="17" t="s">
         <v>68</v>
@@ -2734,8 +2723,27 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J34" t="s">
+        <v>271</v>
+      </c>
+      <c r="L34" s="24">
+        <f>'TIG Welder'!F6+'TIG Welder'!F7</f>
+        <v>196</v>
+      </c>
+      <c r="M34">
+        <v>2</v>
+      </c>
+      <c r="N34" s="24">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>58</v>
       </c>
@@ -2753,11 +2761,30 @@
         <f t="shared" si="0"/>
         <v>1238.8902659254277</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" t="s">
+        <v>293</v>
+      </c>
+      <c r="J35" t="s">
+        <v>271</v>
+      </c>
+      <c r="L35" s="24">
+        <f>'TIG Welder'!F5</f>
+        <v>8579</v>
+      </c>
+      <c r="M35">
+        <v>10</v>
+      </c>
+      <c r="N35" s="24">
+        <f t="shared" si="2"/>
+        <v>857.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C36" s="24">
         <f>'Tooling and small machinery'!F6*2+'Tooling and small machinery'!F7*2</f>
@@ -2770,8 +2797,30 @@
         <f t="shared" si="0"/>
         <v>542.49680000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" t="s">
+        <v>271</v>
+      </c>
+      <c r="K36" t="s">
+        <v>307</v>
+      </c>
+      <c r="L36" s="24">
+        <f>0.03*(L31+L32)</f>
+        <v>275.04599999999999</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36" s="24">
+        <f t="shared" si="2"/>
+        <v>275.04599999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" t="s">
         <v>63</v>
@@ -2783,13 +2832,24 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" t="s">
+        <v>272</v>
+      </c>
+      <c r="K37" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -2798,17 +2858,41 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="48" t="s">
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" t="s">
+        <v>38</v>
+      </c>
+      <c r="J38" t="s">
+        <v>272</v>
+      </c>
+      <c r="K38" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" t="s">
+        <v>295</v>
+      </c>
+      <c r="J39" t="s">
+        <v>272</v>
+      </c>
+      <c r="K39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
       <c r="D41" s="36"/>
       <c r="E41" s="36"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>39</v>
       </c>
@@ -2819,11 +2903,11 @@
         <v>73</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E42" s="19"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -2837,7 +2921,7 @@
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>75</v>
       </c>
@@ -2848,7 +2932,7 @@
       <c r="D44" s="24"/>
       <c r="E44" s="24"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>76</v>
       </c>
@@ -2859,7 +2943,7 @@
       <c r="D45" s="24"/>
       <c r="E45" s="24"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>77</v>
       </c>
@@ -2870,7 +2954,7 @@
       <c r="D46" s="24"/>
       <c r="E46" s="24"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -2881,7 +2965,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>80</v>
       </c>
@@ -2900,25 +2984,25 @@
         <v>0.75</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E49" s="28"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C50" s="28">
         <v>0.9</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E50" s="28"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C51" s="41">
         <f>C48*C47*C49*C57</f>
@@ -2935,7 +3019,7 @@
         <v>205</v>
       </c>
       <c r="C52" s="24">
-        <f>Energies!B5</f>
+        <f>Energies!B6</f>
         <v>2843.9040000000005</v>
       </c>
       <c r="D52" s="24"/>
@@ -2946,7 +3030,7 @@
         <v>206</v>
       </c>
       <c r="C53" s="33">
-        <f>Energies!B6</f>
+        <f>Energies!B7</f>
         <v>7.8299999999999995E-2</v>
       </c>
       <c r="D53" s="37"/>
@@ -2976,13 +3060,31 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C57">
         <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>312</v>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>356</v>
+      </c>
+      <c r="C58" s="25">
+        <f>SUM(E3:E38)</f>
+        <v>122669.88090523001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>357</v>
+      </c>
+      <c r="C59" s="25">
+        <f>C58/SUM(Manpower!B26:I26)</f>
+        <v>12.497695550383073</v>
       </c>
     </row>
   </sheetData>
@@ -3097,7 +3199,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CCC6EF-A592-4848-BAEA-E441E8495A29}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -3116,37 +3218,47 @@
         <v>203</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>347</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>344</v>
-      </c>
-      <c r="B3">
-        <v>38.64</v>
+      <c r="B3" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B4">
-        <f>24*0.8*3+16</f>
-        <v>73.600000000000009</v>
+        <v>38.64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>344</v>
       </c>
-      <c r="B5" s="2">
-        <f>B4*B3</f>
-        <v>2843.9040000000005</v>
+      <c r="B5">
+        <f>24*0.8*3+16</f>
+        <v>73.600000000000009</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B6" s="2">
+        <f>B5*B4</f>
+        <v>2843.9040000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>204</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B7" s="30">
         <v>7.8299999999999995E-2</v>
       </c>
     </row>
@@ -3466,30 +3578,30 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>297</v>
+      </c>
+      <c r="B23" t="s">
         <v>298</v>
-      </c>
-      <c r="B23" t="s">
-        <v>299</v>
       </c>
       <c r="E23" s="2">
         <v>48334.81</v>
       </c>
       <c r="F23" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>301</v>
+      </c>
+      <c r="B25" t="s">
         <v>302</v>
-      </c>
-      <c r="B25" t="s">
-        <v>303</v>
       </c>
       <c r="E25" s="2">
         <v>5390</v>
       </c>
       <c r="F25" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -3521,13 +3633,13 @@
         <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E1" t="s">
         <v>249</v>
@@ -3589,10 +3701,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6" t="s">
         <v>285</v>
-      </c>
-      <c r="B6" t="s">
-        <v>286</v>
       </c>
       <c r="C6" s="22"/>
       <c r="F6" s="2">
@@ -3604,10 +3716,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C7" s="22"/>
       <c r="E7" s="2">
@@ -3677,7 +3789,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B26" sqref="B26:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3722,16 +3834,16 @@
         <v>194</v>
       </c>
       <c r="D4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G4" t="s">
+        <v>330</v>
+      </c>
+      <c r="H4" t="s">
         <v>331</v>
-      </c>
-      <c r="H4" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3762,7 +3874,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B6" s="2">
         <v>2438</v>
@@ -3788,7 +3900,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B7" s="2">
         <v>4104</v>
@@ -3814,7 +3926,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F8">
         <f>SUM(F7+F6+F5)</f>
@@ -3885,25 +3997,25 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>320</v>
+      </c>
+      <c r="C21" t="s">
         <v>321</v>
-      </c>
-      <c r="C21" t="s">
-        <v>322</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
       </c>
       <c r="E21" t="s">
+        <v>322</v>
+      </c>
+      <c r="F21" t="s">
         <v>323</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>324</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>325</v>
-      </c>
-      <c r="H21" t="s">
-        <v>326</v>
       </c>
       <c r="I21" t="s">
         <v>40</v>
@@ -3912,7 +4024,7 @@
         <v>27</v>
       </c>
       <c r="K21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3947,7 +4059,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F23">
         <v>0.9</v>
@@ -3971,7 +4083,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H24">
         <v>0.3</v>
@@ -3989,42 +4101,42 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B25">
-        <f>$B$28*SUM(B22:B24)</f>
+        <f t="shared" ref="B25:J25" si="2">$B$28*SUM(B22:B24)</f>
         <v>1220.9399999999998</v>
       </c>
       <c r="C25">
-        <f>$B$28*SUM(C22:C24)</f>
+        <f t="shared" si="2"/>
         <v>1220.9399999999998</v>
       </c>
       <c r="D25">
-        <f>$B$28*SUM(D22:D24)</f>
+        <f t="shared" si="2"/>
         <v>1220.9399999999998</v>
       </c>
       <c r="E25">
-        <f>$B$28*SUM(E22:E24)</f>
+        <f t="shared" si="2"/>
         <v>1220.9399999999998</v>
       </c>
       <c r="F25">
-        <f>$B$28*SUM(F22:F24)</f>
+        <f t="shared" si="2"/>
         <v>1292.76</v>
       </c>
       <c r="G25">
-        <f>$B$28*SUM(G22:G24)</f>
+        <f t="shared" si="2"/>
         <v>1292.76</v>
       </c>
       <c r="H25">
-        <f>$B$28*SUM(H22:H24)</f>
+        <f t="shared" si="2"/>
         <v>1292.76</v>
       </c>
       <c r="I25">
-        <f>$B$28*SUM(I22:I24)</f>
+        <f t="shared" si="2"/>
         <v>1580.0399999999997</v>
       </c>
       <c r="J25">
-        <f>$B$28*SUM(J22:J24)</f>
+        <f t="shared" si="2"/>
         <v>574.55999999999995</v>
       </c>
       <c r="K25">
@@ -4034,7 +4146,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B26">
         <f>General!$C$49*General!$C$48*General!$C$47</f>
@@ -4079,7 +4191,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B28">
         <f>General!$C$50*General!$C$48*General!$C$47</f>
@@ -4088,7 +4200,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B30" s="24">
         <f>SUMPRODUCT(D5:D7*J22:J24)</f>
@@ -4130,13 +4242,13 @@
         <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E1" t="s">
         <v>249</v>
@@ -4161,13 +4273,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F3" s="2">
         <v>922.6</v>
       </c>
       <c r="G3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4178,7 +4290,7 @@
         <v>3859.6</v>
       </c>
       <c r="G4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>